<commit_message>
Everything is wrong, don't do anything
</commit_message>
<xml_diff>
--- a/Database Creation/SampleDataSuperheroSightings.xlsx
+++ b/Database Creation/SampleDataSuperheroSightings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shazena\Documents\GITHUB\DDWAM4A-SuperheroSightings\Database Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526FF1BF-C451-4DBE-ADBD-939942159740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86E0ED5-C3D8-48AE-ACF5-7524B638ECDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E8F90E5-34C3-4543-8015-63099B1EBA72}"/>
   </bookViews>
@@ -478,6 +478,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,11 +491,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6C6B24-9F23-403D-8EEA-51F41BC2ED7D}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="78" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,12 +830,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G2" s="13" t="s">
@@ -906,12 +906,12 @@
       <c r="J6" s="4">
         <v>44014</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="5">
@@ -982,17 +982,17 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
+      <c r="B11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
       <c r="N11" s="1">
         <v>4</v>
       </c>
@@ -1078,10 +1078,10 @@
       <c r="N13" s="1">
         <v>6</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="18" t="s">
         <v>94</v>
       </c>
       <c r="Q13" s="3">
@@ -1119,10 +1119,10 @@
       <c r="N14" s="5">
         <v>7</v>
       </c>
-      <c r="O14" s="22" t="s">
+      <c r="O14" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="P14" s="19" t="s">
         <v>97</v>
       </c>
       <c r="Q14" s="8">
@@ -1154,32 +1154,32 @@
       <c r="I15" s="6">
         <v>41.874589</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="O20" s="18" t="s">
+      <c r="L20" s="23"/>
+      <c r="O20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="P20" s="20"/>
+      <c r="P20" s="23"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="20"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="23"/>
       <c r="K21" s="13" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Had to change an address that MySQL Workbench didn't like
</commit_message>
<xml_diff>
--- a/Database Creation/SampleDataSuperheroSightings.xlsx
+++ b/Database Creation/SampleDataSuperheroSightings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shazena\Documents\GITHUB\DDWAM4A-SuperheroSightings\Database Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8F325A-6501-4C3A-9D88-72A39D55A356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2CE48D-DB43-4D35-B1FB-FA2F99A11236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E8F90E5-34C3-4543-8015-63099B1EBA72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
   <si>
     <t>id</t>
   </si>
@@ -197,24 +197,9 @@
     <t>MA</t>
   </si>
   <si>
-    <t>STAT Analysis Corporation</t>
-  </si>
-  <si>
     <t>Lab</t>
   </si>
   <si>
-    <t>2242 W Harrison St Suite 200</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t> -87.683031</t>
-  </si>
-  <si>
     <t>Earth’s first line of defense against threats too large for humanity to face alone</t>
   </si>
   <si>
@@ -321,6 +306,18 @@
   </si>
   <si>
     <t>550 Main St</t>
+  </si>
+  <si>
+    <t>Labcorp</t>
+  </si>
+  <si>
+    <t>Beckley</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>406 Carriage Dr</t>
   </si>
 </sst>
 </file>
@@ -470,15 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,6 +486,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6C6B24-9F23-403D-8EEA-51F41BC2ED7D}">
   <dimension ref="B1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="90" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,12 +833,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G2" s="12" t="s">
@@ -912,12 +909,12 @@
       <c r="J6" s="4">
         <v>44014</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="5">
@@ -933,7 +930,7 @@
         <v>43845</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O7" s="15" t="s">
         <v>5</v>
@@ -942,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
@@ -974,17 +971,17 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
+      <c r="B10" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29"/>
       <c r="N10" s="1">
         <v>3</v>
       </c>
@@ -1112,10 +1109,10 @@
         <v>6</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="Q13" s="3">
         <v>5</v>
@@ -1126,62 +1123,62 @@
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="H14" s="9">
-        <v>60612</v>
+        <v>25801</v>
       </c>
       <c r="I14" s="2">
-        <v>41.874589</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>59</v>
+        <v>37.787906</v>
+      </c>
+      <c r="J14" s="21">
+        <v>-81.199005999999997</v>
       </c>
       <c r="N14" s="5">
         <v>7</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="Q14" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="23">
+      <c r="B15" s="20">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>11215</v>
       </c>
       <c r="I15" s="2">
@@ -1192,25 +1189,25 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="23">
+      <c r="B16" s="20">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D16" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>89</v>
-      </c>
       <c r="G16" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="22">
+        <v>61</v>
+      </c>
+      <c r="H16" s="19">
         <v>90004</v>
       </c>
       <c r="I16" s="2">
@@ -1221,25 +1218,25 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="23">
+      <c r="B17" s="20">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="22">
+        <v>62</v>
+      </c>
+      <c r="H17" s="19">
         <v>77590</v>
       </c>
       <c r="I17" s="2">
@@ -1250,25 +1247,25 @@
       </c>
     </row>
     <row r="18" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="25">
+      <c r="B18" s="22">
         <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="26">
+        <v>89</v>
+      </c>
+      <c r="H18" s="23">
         <v>6615</v>
       </c>
       <c r="I18" s="6">
@@ -1280,7 +1277,7 @@
     </row>
     <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="21"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1289,14 +1286,14 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="O20" s="18" t="s">
+      <c r="L20" s="29"/>
+      <c r="O20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="P20" s="20"/>
+      <c r="P20" s="29"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K21" s="12" t="s">
@@ -1306,7 +1303,7 @@
         <v>18</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="P21" s="14" t="s">
         <v>19</v>
@@ -1494,17 +1491,17 @@
     </row>
     <row r="43" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="20"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>5</v>
@@ -1513,9 +1510,9 @@
         <v>6</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1527,7 +1524,7 @@
         <v>21</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E46" s="2">
         <v>1111111111</v>
@@ -1544,7 +1541,7 @@
         <v>22</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E47" s="2">
         <v>2222222222</v>
@@ -1561,7 +1558,7 @@
         <v>23</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E48" s="2">
         <v>3333333333</v>
@@ -1578,7 +1575,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E49" s="2">
         <v>4444444444</v>
@@ -1595,7 +1592,7 @@
         <v>26</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E50" s="2">
         <v>5555555555</v>
@@ -1612,7 +1609,7 @@
         <v>29</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E51" s="2">
         <v>6666666666</v>
@@ -1629,12 +1626,12 @@
         <v>27</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E52" s="2">
         <v>7777777777</v>
       </c>
-      <c r="F52" s="28">
+      <c r="F52" s="25">
         <v>6</v>
       </c>
     </row>
@@ -1646,12 +1643,12 @@
         <v>32</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E53" s="6">
         <v>8888888888</v>
       </c>
-      <c r="F53" s="29">
+      <c r="F53" s="26">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor updates made - column names corrected
</commit_message>
<xml_diff>
--- a/Database Creation/SampleDataSuperheroSightings.xlsx
+++ b/Database Creation/SampleDataSuperheroSightings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shazena\Documents\GITHUB\DDWAM4A-SuperheroSightings\Database Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2CE48D-DB43-4D35-B1FB-FA2F99A11236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBC7EC5-FD1C-4071-B128-72C6AA0B0F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E8F90E5-34C3-4543-8015-63099B1EBA72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
     <t>id</t>
   </si>
@@ -86,12 +86,6 @@
     <t>powersuper</t>
   </si>
   <si>
-    <t>superName</t>
-  </si>
-  <si>
-    <t>organizationName</t>
-  </si>
-  <si>
     <t>powerName</t>
   </si>
   <si>
@@ -318,14 +312,30 @@
   </si>
   <si>
     <t>406 Carriage Dr</t>
+  </si>
+  <si>
+    <t>SuperheroId</t>
+  </si>
+  <si>
+    <t>OrgId</t>
+  </si>
+  <si>
+    <t>superheroId</t>
+  </si>
+  <si>
+    <t>superheroName</t>
+  </si>
+  <si>
+    <t>orgName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00000"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -441,10 +451,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -495,6 +503,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6C6B24-9F23-403D-8EEA-51F41BC2ED7D}">
   <dimension ref="B1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="90" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,24 +843,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -858,13 +868,13 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
+      <c r="H3" s="2">
+        <v>4</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="28">
         <v>44055</v>
       </c>
     </row>
@@ -872,13 +882,13 @@
       <c r="G4" s="1">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
+      <c r="H4" s="2">
+        <v>2</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="28">
         <v>44055</v>
       </c>
     </row>
@@ -886,13 +896,13 @@
       <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>31</v>
+      <c r="H5" s="2">
+        <v>1</v>
       </c>
       <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="28">
         <v>44014</v>
       </c>
     </row>
@@ -900,46 +910,46 @@
       <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>30</v>
+      <c r="H6" s="2">
+        <v>5</v>
       </c>
       <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="28">
         <v>44014</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="27"/>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>5</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="H7" s="5">
         <v>3</v>
       </c>
-      <c r="J7" s="7">
+      <c r="I7" s="5">
+        <v>3</v>
+      </c>
+      <c r="J7" s="29">
         <v>43845</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="P7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
@@ -947,10 +957,10 @@
         <v>1</v>
       </c>
       <c r="O8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="Q8" s="3">
         <v>1</v>
@@ -961,101 +971,101 @@
         <v>2</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
+      <c r="B10" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
       <c r="N10" s="1">
         <v>3</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q10" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="12" t="s">
         <v>12</v>
       </c>
       <c r="N11" s="1">
         <v>4</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q11" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <v>13088</v>
       </c>
       <c r="I12" s="2">
@@ -1068,35 +1078,35 @@
         <v>5</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>1760</v>
       </c>
       <c r="I13" s="2">
@@ -1108,77 +1118,77 @@
       <c r="N13" s="1">
         <v>6</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>69</v>
+      <c r="O13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="Q13" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <v>25801</v>
       </c>
       <c r="I14" s="2">
         <v>37.787906</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="19">
         <v>-81.199005999999997</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="4">
         <v>7</v>
       </c>
-      <c r="O14" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="P14" s="17" t="s">
+      <c r="O14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="18">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Q14" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="20">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="F15" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="19">
+      <c r="G15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="17">
         <v>11215</v>
       </c>
       <c r="I15" s="2">
@@ -1189,25 +1199,25 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="20">
+      <c r="B16" s="18">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="19">
+        <v>83</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="17">
         <v>90004</v>
       </c>
       <c r="I16" s="2">
@@ -1218,25 +1228,25 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="20">
+      <c r="B17" s="18">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="19">
+        <v>60</v>
+      </c>
+      <c r="H17" s="17">
         <v>77590</v>
       </c>
       <c r="I17" s="2">
@@ -1247,37 +1257,37 @@
       </c>
     </row>
     <row r="18" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>7</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="G18" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="23">
+      <c r="H18" s="21">
         <v>6615</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>41.17118</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="6">
         <v>-73.125349</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1286,27 +1296,27 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="27" t="s">
+      <c r="K20" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="29"/>
-      <c r="O20" s="27" t="s">
+      <c r="L20" s="27"/>
+      <c r="O20" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="P20" s="29"/>
+      <c r="P20" s="27"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="P21" s="14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
@@ -1320,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
@@ -1334,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
@@ -1348,7 +1358,7 @@
         <v>3</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
@@ -1362,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1376,7 +1386,7 @@
         <v>5</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="52.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1386,11 +1396,11 @@
       <c r="L27" s="3">
         <v>4</v>
       </c>
-      <c r="O27" s="5">
+      <c r="O27" s="4">
         <v>6</v>
       </c>
-      <c r="P27" s="8" t="s">
-        <v>34</v>
+      <c r="P27" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -1482,37 +1492,37 @@
       </c>
     </row>
     <row r="39" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K39" s="5">
+      <c r="K39" s="4">
         <v>7</v>
       </c>
-      <c r="L39" s="8">
+      <c r="L39" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="29"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="27"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" s="24" t="s">
+      <c r="E45" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1521,10 +1531,10 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>56</v>
+        <v>19</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E46" s="2">
         <v>1111111111</v>
@@ -1538,10 +1548,10 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>55</v>
+        <v>20</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="E47" s="2">
         <v>2222222222</v>
@@ -1555,10 +1565,10 @@
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="E48" s="2">
         <v>3333333333</v>
@@ -1572,10 +1582,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>58</v>
+        <v>23</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="E49" s="2">
         <v>4444444444</v>
@@ -1589,10 +1599,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>64</v>
+        <v>24</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="E50" s="2">
         <v>5555555555</v>
@@ -1606,10 +1616,10 @@
         <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>59</v>
+        <v>27</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="E51" s="2">
         <v>6666666666</v>
@@ -1623,32 +1633,32 @@
         <v>7</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="E52" s="2">
         <v>7777777777</v>
       </c>
-      <c r="F52" s="25">
+      <c r="F52" s="23">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="5">
+      <c r="B53" s="4">
         <v>8</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53" s="6">
+      <c r="C53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="5">
         <v>8888888888</v>
       </c>
-      <c r="F53" s="26">
+      <c r="F53" s="24">
         <v>6</v>
       </c>
     </row>

</xml_diff>